<commit_message>
Stability improvements, modification to the data processing to fix a crashing issue, and initial stab at Khmer language integration.
</commit_message>
<xml_diff>
--- a/agquery/Update/evidence_list.xlsx
+++ b/agquery/Update/evidence_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C023E644-EC6A-4D48-9B0D-68E4A35C18D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46032328-0683-4E24-88AC-0FE309773D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{1AFB0CF4-0FB3-4D51-9152-4D06EA205B7D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1AFB0CF4-0FB3-4D51-9152-4D06EA205B7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
-  <si>
-    <t>Evidence</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Poultry</t>
   </si>
@@ -108,16 +105,90 @@
   </si>
   <si>
     <t>Olmo, L., Ashley, K., Young, J.R., et al. (2017). Improving smallholder cattle reproductive efficiency in Cambodia to address expanding regional beef demand. Tropical Animal Health and Production, 49(1), 163-172. https://doi.org/10.1007/s11250-016-1175-6</t>
+  </si>
+  <si>
+    <t>https://www.publish.csiro.au/an/AN16164</t>
+  </si>
+  <si>
+    <t>https://www.publish.csiro.au/an/an14133</t>
+  </si>
+  <si>
+    <t>https://www.publish.csiro.au/an/an14136</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/abs/10.1080/14728028.2020.1827049</t>
+  </si>
+  <si>
+    <t>https://www.aciar.gov.au/sites/default/files/2023-03/LPS-2015-037-final-report_0.pdf</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1002/vms3.1191</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1111/j.1865-1682.2011.01247.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://link.springer.com/article/10.1007/s11250-016-1175-6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://link.springer.com/article/10.1007/s13593-019-0576-0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://link.springer.com/article/10.1007/s11250-015-0863-y </t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1111/tbed.14317</t>
+  </si>
+  <si>
+    <t>https://www.aciar.gov.au/sites/default/files/project-page-docs/final_report_ah-2010-046.pdf</t>
+  </si>
+  <si>
+    <t>https://policycommons.net/artifacts/3883852/testing-innovative-approaches-to-extension-in-cambodia/4690127/</t>
+  </si>
+  <si>
+    <t>https://cgspace.cgiar.org/items/21268e89-4470-4d91-9bba-57dbdae4e173</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/abs/10.1080/00439339.2021.1893620</t>
+  </si>
+  <si>
+    <t>https://cgspace.cgiar.org/server/api/core/bitstreams/d83e6a0b-0a95-40bc-855b-f1b6e576dfcd/content</t>
+  </si>
+  <si>
+    <t>https://cgspace.cgiar.org/server/api/core/bitstreams/ded9c4dc-48ac-4d70-b16b-5e500ca4a1d6/content</t>
+  </si>
+  <si>
+    <t>https://resources.peopleinneed.net/documents/12-pin-barrier-analysis-studies-electronicv.pdf</t>
+  </si>
+  <si>
+    <t>https://journals.sagepub.com/doi/abs/10.1177/156482651303400206</t>
+  </si>
+  <si>
+    <t>https://cgspace.cgiar.org/items/53477955-1acb-4741-93ec-241bf2102bcd</t>
+  </si>
+  <si>
+    <t>Citation</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,13 +211,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,184 +556,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2AE4825-5FB4-4C86-AB8A-7CEBB3E397EA}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="149.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C20" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4</v>
+      <c r="C21" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -664,6 +804,29 @@
     <sortCondition ref="A2:A21"/>
     <sortCondition ref="B2:B21"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{7DC566EE-1F41-40D8-98A4-4F4824B8E783}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{83B44B32-600A-4045-A1AA-DD1C04AB65BA}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{A428BD06-E2BF-4FF8-A4C9-9AD04EDCE228}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{6A75FD6F-7A1F-4308-94FB-E86E4AF2AD82}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{5EFD73B8-7253-4103-B437-A428E4C3DBB9}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{F96CEF8B-2D10-4C69-93C0-E25AF975A90A}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{D06F5F5C-44CB-48C1-ABB6-0A3D9F2E9ED9}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{A59D92AB-FA2A-4ED9-ABCA-CC844D66A27D}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{DE53F991-3DCB-4171-9E9B-05765464990B}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{13F1B864-97F6-496D-AE4D-F3475E9565AE}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{B14AD7FB-79D3-4CDE-AFA1-28B3D905C7DB}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{54CB2DA7-B897-496F-9E93-80450730B3B7}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{3EEFDED9-7116-435D-93C0-8BEB34CE8FDD}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{68C74387-E554-450C-AA94-1B0451F4EC77}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{6726CD9D-3EF4-4D01-B9AA-660F9C349F48}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{19330DF6-034C-4A8F-844F-B16C18E20863}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{2DEA290B-60D3-4E2D-A10F-FFD54E2045B4}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{1F1AFBE6-730C-4FE5-B3BF-A31CB2D71158}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{83D3D379-0727-4175-84D2-03688FB34890}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{0DAD4EAC-31B9-4248-8BC7-6B1F0BFD91FE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>